<commit_message>
sagarrokade: create new sheet in excel
</commit_message>
<xml_diff>
--- a/type of lookup.xlsx
+++ b/type of lookup.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\da18\Excel\day-8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\da18\github data\da18ExcelTask2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D17F69-64C5-494B-96C9-666AA90D829C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F55B22A-710F-4432-8FE0-0B6FFBE0CAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="date func" sheetId="4" r:id="rId2"/>
+    <sheet name="test" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -964,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB088D21-2000-4B72-B600-29409BD5F1F2}">
   <dimension ref="D4:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="136" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="136" workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
@@ -1011,7 +1012,7 @@
       </c>
       <c r="I10" s="3">
         <f ca="1">NOW()</f>
-        <v>45752.371715162037</v>
+        <v>45752.420930787041</v>
       </c>
     </row>
     <row r="12" spans="6:11" x14ac:dyDescent="0.3">
@@ -1020,7 +1021,7 @@
       </c>
       <c r="I12" s="3">
         <f ca="1">I10-2.343</f>
-        <v>45750.028715162036</v>
+        <v>45750.07793078704</v>
       </c>
     </row>
     <row r="15" spans="6:11" x14ac:dyDescent="0.3">
@@ -1029,7 +1030,7 @@
       </c>
       <c r="I15" s="4">
         <f ca="1">I10</f>
-        <v>45752.371715162037</v>
+        <v>45752.420930787041</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.3">
@@ -1038,7 +1039,7 @@
       </c>
       <c r="I17" s="5">
         <f ca="1">I15</f>
-        <v>45752.371715162037</v>
+        <v>45752.420930787041</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.3">
@@ -1159,4 +1160,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54865BC0-F190-46A6-A798-5C55721DA5E0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>